<commit_message>
Pooh Points: normal 20260207
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-07.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-07.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,13 +428,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -564,6 +564,1318 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Boozers Losers</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Billy Richmond III</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>5</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>The Backslashers</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Trevon Brazile</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3</v>
+      </c>
+      <c r="R3" t="n">
+        <v>4</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>The Backslashers</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Meleek Thomas</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>The Backslashers</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Jayden Epps</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hilton Heads</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Quincy Ballard</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Three Dawg Nite</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Nick Pringle</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bend Rimmers</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Darius Acuff Jr.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>G-Flop</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Josh Hubbard</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>The Oddities</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Shawn Jones Jr.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Achor Achor</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>3</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Malique Ewin</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>4</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Isaiah Sealy</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Ja'Borri McGhee</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Jamarion Davis-Fleming</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>King Grace</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sergej Macura</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>MSST</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>ARK@MSST</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>13:06 - 1st Half</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>-3</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -575,7 +1887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +1895,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
   </cols>
@@ -605,6 +1917,97 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The Backslashers</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bend Rimmers</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Boozers Losers</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hilton Heads</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Three Dawg Nite</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>G-Flop</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The Oddities</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Pooh Points: final 20260207 -> PD11
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-07.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-07.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -679,7 +679,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H36" t="n">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H38" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -4123,7 +4123,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H50" t="n">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H58" t="n">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H62" t="n">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H66" t="n">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H70" t="n">
@@ -6829,7 +6829,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H78" t="n">
@@ -7157,7 +7157,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H82" t="n">
@@ -7239,7 +7239,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H83" t="n">
@@ -7485,7 +7485,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H86" t="n">
@@ -7895,7 +7895,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H91" t="n">
@@ -8141,7 +8141,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -8387,7 +8387,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H97" t="n">
@@ -8633,7 +8633,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H100" t="n">
@@ -9453,7 +9453,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H110" t="n">
@@ -9945,7 +9945,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -10027,7 +10027,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -10273,7 +10273,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -10519,7 +10519,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -10847,7 +10847,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H127" t="n">
@@ -11585,7 +11585,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H136" t="n">
@@ -11667,7 +11667,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H137" t="n">
@@ -11749,7 +11749,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H138" t="n">
@@ -11831,7 +11831,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H139" t="n">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>6:33 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H145" t="n">
@@ -12815,7 +12815,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -12897,7 +12897,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>3:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H152" t="n">

</xml_diff>